<commit_message>
Completed the rules aspect
</commit_message>
<xml_diff>
--- a/Xero Reconciliation Robot Chrome Version/Data/Config.xlsx
+++ b/Xero Reconciliation Robot Chrome Version/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\UiPath_Project\Xero Reconciliation Robot Chrome Version\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF01DBB-7DE1-4C27-990F-42799F49266E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4022009B-12C1-428A-983D-57DC6FE4AE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2879,7 +2879,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>